<commit_message>
Fun times it is now time to start the analysis workflow over again at 01.R because now I've made manual edits in Excel to integrate info in Notes columns into the data
</commit_message>
<xml_diff>
--- a/Sonoran-data/raw/from-Master_species-list-with-native-status_LO.xlsx
+++ b/Sonoran-data/raw/from-Master_species-list-with-native-status_LO.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://emailarizona-my.sharepoint.com/personal/lossanna_arizona_edu/Documents/grad school/Gornish lab/04_RAMPS RestoreNet/RestoreNet/data/raw/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://eltnmsu-my.sharepoint.com/personal/lossanna_nmsu_edu/Documents/Documents/02_RestoreNet/RestoreNet/Sonoran-data/raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1748" documentId="8_{FF5EA2F2-2FF6-42D4-ADD7-A9144DE3C437}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FA96F209-A0CC-45CA-8A47-38142C1D367E}"/>
+  <xr:revisionPtr revIDLastSave="1749" documentId="8_{FF5EA2F2-2FF6-42D4-ADD7-A9144DE3C437}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5D1E8554-A1C8-45A2-A806-4D1BA2F09BF7}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="25440" windowHeight="15270" xr2:uid="{6ED14566-95D0-4DF3-9156-CD80DAE02F6C}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{6ED14566-95D0-4DF3-9156-CD80DAE02F6C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -2472,16 +2472,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>15240</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>15240</xdr:rowOff>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>251460</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>53340</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>129540</xdr:colOff>
-      <xdr:row>15</xdr:row>
-      <xdr:rowOff>28575</xdr:rowOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>365760</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -2496,8 +2496,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="11292840" y="377190"/>
-          <a:ext cx="4352925" cy="2366010"/>
+          <a:off x="10302240" y="784860"/>
+          <a:ext cx="4351020" cy="2390775"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2592,9 +2592,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -2632,7 +2632,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -2738,7 +2738,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -2880,7 +2880,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -2932,8 +2932,8 @@
   <dimension ref="A1:D473"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A452" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A470" sqref="A470"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H441" sqref="H441"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Begin on rerunning 01.R after doing manual Excel edits (although a lot of the edits on the Sonoran SE subplot codes were unnecessary because they were already keyed to the species list, so then I had to go back and undo those lol)
</commit_message>
<xml_diff>
--- a/Sonoran-data/raw/from-Master_species-list-with-native-status_LO.xlsx
+++ b/Sonoran-data/raw/from-Master_species-list-with-native-status_LO.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://eltnmsu-my.sharepoint.com/personal/lossanna_nmsu_edu/Documents/Documents/02_RestoreNet/RestoreNet/Sonoran-data/raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1749" documentId="8_{FF5EA2F2-2FF6-42D4-ADD7-A9144DE3C437}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5D1E8554-A1C8-45A2-A806-4D1BA2F09BF7}"/>
+  <xr:revisionPtr revIDLastSave="1751" documentId="8_{FF5EA2F2-2FF6-42D4-ADD7-A9144DE3C437}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{507D0AB6-8F78-44D7-BB8A-237FAEED50D7}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{6ED14566-95D0-4DF3-9156-CD80DAE02F6C}"/>
   </bookViews>
@@ -2932,8 +2932,8 @@
   <dimension ref="A1:D473"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H441" sqref="H441"/>
+      <pane ySplit="1" topLeftCell="A275" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A298" sqref="A298"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6859,7 +6859,7 @@
         <v>444</v>
       </c>
       <c r="C280" t="s">
-        <v>16</v>
+        <v>205</v>
       </c>
       <c r="D280" t="s">
         <v>2</v>
@@ -6999,7 +6999,7 @@
         <v>454</v>
       </c>
       <c r="C290" t="s">
-        <v>16</v>
+        <v>7</v>
       </c>
       <c r="D290" t="s">
         <v>2</v>

</xml_diff>